<commit_message>
updates spreadshhet with HFOV findings
</commit_message>
<xml_diff>
--- a/ROSORPlugins/PETER_ROSOR_flightline_creator/Typical-Required-overlap-line-spacing.xlsx
+++ b/ROSORPlugins/PETER_ROSOR_flightline_creator/Typical-Required-overlap-line-spacing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t xml:space="preserve">Drone</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">60-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HFOV with 24 mm lens is calculated and measured to be closer to 75 degreees, somwhere between 82 and the 72</t>
   </si>
 </sst>
 </file>
@@ -155,15 +158,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>271440</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:colOff>459000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>207000</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:colOff>394200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -176,8 +179,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="271440" y="897480"/>
-          <a:ext cx="5487840" cy="3584520"/>
+          <a:off x="459000" y="1238400"/>
+          <a:ext cx="5487120" cy="3584160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -197,10 +200,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -262,6 +265,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D33" s="0"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>